<commit_message>
Fix typo excel algorithme
</commit_message>
<xml_diff>
--- a/files/autodiag/algorithme.xlsx
+++ b/files/autodiag/algorithme.xlsx
@@ -20,7 +20,7 @@
     <t>algorithme</t>
   </si>
   <si>
-    <t>libelle_valeur_referece_1</t>
+    <t>libelle_valeur_reference_1</t>
   </si>
   <si>
     <t>calcul_valeur_reference_1</t>
@@ -29,7 +29,7 @@
     <t>couleur_reference_1</t>
   </si>
   <si>
-    <t>libelle_valeur_referece_2</t>
+    <t>libelle_valeur_reference_2</t>
   </si>
   <si>
     <t>calcul_valeur_reference_2</t>
@@ -38,7 +38,7 @@
     <t>couleur_reference_2</t>
   </si>
   <si>
-    <t>libelle_valeur_referece_3</t>
+    <t>libelle_valeur_reference_3</t>
   </si>
   <si>
     <t>calcul_valeur_reference_3</t>
@@ -47,7 +47,7 @@
     <t>couleur_reference_3</t>
   </si>
   <si>
-    <t>libelle_valeur_referece_4</t>
+    <t>libelle_valeur_reference_4</t>
   </si>
   <si>
     <t>calcul_valeur_reference_4</t>
@@ -56,7 +56,7 @@
     <t>couleur_reference_4</t>
   </si>
   <si>
-    <t>libelle_valeur_referece_5</t>
+    <t>libelle_valeur_reference_5</t>
   </si>
   <si>
     <t>calcul_valeur_reference_5</t>
@@ -65,7 +65,7 @@
     <t>couleur_reference_5</t>
   </si>
   <si>
-    <t>libelle_valeur_referece_6</t>
+    <t>libelle_valeur_reference_6</t>
   </si>
   <si>
     <t>calcul_valeur_reference_6</t>
@@ -74,7 +74,7 @@
     <t>couleur_reference_6</t>
   </si>
   <si>
-    <t>libelle_valeur_referece_7</t>
+    <t>libelle_valeur_reference_7</t>
   </si>
   <si>
     <t>calcul_valeur_reference_7</t>
@@ -83,7 +83,7 @@
     <t>couleur_reference_7</t>
   </si>
   <si>
-    <t>libelle_valeur_referece_8</t>
+    <t>libelle_valeur_reference_8</t>
   </si>
   <si>
     <t>calcul_valeur_reference_8</t>
@@ -92,7 +92,7 @@
     <t>couleur_reference_8</t>
   </si>
   <si>
-    <t>libelle_valeur_referece_9</t>
+    <t>libelle_valeur_reference_9</t>
   </si>
   <si>
     <t>calcul_valeur_reference_9</t>
@@ -101,7 +101,7 @@
     <t>couleur_reference_9</t>
   </si>
   <si>
-    <t>libelle_valeur_referece_10</t>
+    <t>libelle_valeur_reference_10</t>
   </si>
   <si>
     <t>calcul_valeur_reference_10</t>
@@ -207,8 +207,8 @@
   </sheetPr>
   <dimension ref="A1:AE1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>